<commit_message>
add new exercises, definitions, update decks/lists, etc.
- updated anki deck and wordlist for Lesson 10. (3rd ed.)
- updated news/info module to purge old messages and update existing ones with new info.
- added new definitions to the dictionary.
- added the following exercises.

# Lesson 10 (3rd ed.)
- Kanji Practice: Stroke Order
- Kanji Vocabulary: 住, 正, and 年
- Kanji Vocabulary: 売, 買, and 町
- Kanji Vocabulary: 長, 道, and 雪
- Kanji Vocabulary: 立, 自, and 夜
- Kanji Vocabulary: 朝 and 持
- Kanji Practice: Antonyms
- Kanji Practice: Fill in the Blanks
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-10.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1525,6 +1525,594 @@
         </is>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>to live</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>住む|すむ</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>住所|じゅうしょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>to immigrate</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>移住する|いじゅうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>New Year</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>お正月|おしょうがつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>right</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>正しい|ただしい</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>noon</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>正午|しょうご</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>correct answer</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>正解|せいかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>third-year student</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>三年生|さんねんせい</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>next year</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>来年|らいねん</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>this year</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>今年|ことし</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>年|とし</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>to sell</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>売る|うる</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>stand; stall</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>売店|ばいてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>vending machine</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>自動販売機|じどうはんばいき</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>to buy</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>買う|かう</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>買い物|かいもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>selling and buying</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>売買|ばいばい</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>town</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>町|まち</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Kitayama town</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>北山町|きたやまちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>mayor of a town</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>町長|ちょうちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>長い|ながい</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>the eldest son</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>長男|ちょうなん</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>company president</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>社長|しゃちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>way; road</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>道|みち</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>calligraphy</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>書道|しょどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>judo</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>柔道|じゅうどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Hokkaido</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>北海道|ほっかいどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>snow</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>雪|ゆき</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>new snow</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>新雪|しんせつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>snowman</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>雪だるま|ゆきだるま</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>to stand</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>立つ|たつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>national university</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>国立大学|こくりつだいがく</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>private high school</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>私立高校|しりつこうこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>oneself</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>自分|じぶん</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>automobile</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>自動車|じどうしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>bicycle</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>自転車|じてんしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>freedom</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>自由|じゆう</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>夜|よる</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>middle of night; midnight</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>夜中|よなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>tonight</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>今夜|こんや</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>dawn</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>夜明け|よあけ</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>morning</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>朝|あさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>this morning</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>今朝|けさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>breakfast</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>朝食|ちょうしょく</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>every morning</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>毎朝|まいあさ</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>to carry; to hold</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>持つ|もつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>to bring</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>持ってくる|もってくる</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>belongings</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>所持品|しょじひん</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>feeling</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>気持ち|きもち</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>